<commit_message>
Retoques finales y agregados Conj de Eq a casos de prueba
</commit_message>
<xml_diff>
--- a/Raiz/Trabajos/Práctico/Trabajo_Practico_11/Casos_de_prueba.xlsx
+++ b/Raiz/Trabajos/Práctico/Trabajo_Practico_11/Casos_de_prueba.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User-PC\Documents\GitHub\2021_ISW_4K3_G3\Raiz\Trabajos\Práctico\Trabajo_Practico_11\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jorge\Desktop\Cursado 2021\ISW\2021_ISW_4K3_G3\Raiz\Trabajos\Práctico\Trabajo_Practico_11\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{643D60A6-7B7F-4646-9135-D25E1D2FBF80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{765A8CF3-827C-4246-BB14-68B9DB466FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="679" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="679" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos_Prueba" sheetId="27" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="179">
   <si>
     <t>TC_001</t>
   </si>
@@ -382,9 +382,6 @@
 Elegir opción de confirmar pedido</t>
   </si>
   <si>
-    <t>Realizar un pedido pagando en efectivo con un monto menor al paga</t>
-  </si>
-  <si>
     <t>Realizar pedido sin especificar dirección</t>
   </si>
   <si>
@@ -662,6 +659,86 @@
 TC_005
 TC_012
 </t>
+  </si>
+  <si>
+    <t>13/10/21 18:00</t>
+  </si>
+  <si>
+    <t>No aplica</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>1,4,8,12,14,
+17,40,44</t>
+  </si>
+  <si>
+    <t>Realizar un pedido pagando en efectivo con un monto menor al pagar</t>
+  </si>
+  <si>
+    <t>1,4,8,12,14,
+20,40,44</t>
+  </si>
+  <si>
+    <t>1,4,8,12,14,
+40,44,59</t>
+  </si>
+  <si>
+    <t>1,4,8,12,13,
+21,25,29,33,40,43</t>
+  </si>
+  <si>
+    <t>1,4,8,12,13,
+21,25,29,33,40,44</t>
+  </si>
+  <si>
+    <t>1,4,8,12,14,
+17,40,43</t>
+  </si>
+  <si>
+    <t>2,4,8,12,14,
+17,40,44</t>
+  </si>
+  <si>
+    <t>3,4,8,12,14,
+17,40,44</t>
+  </si>
+  <si>
+    <t>3,4,9,12,14,
+17,40,44</t>
+  </si>
+  <si>
+    <t>1,4,8,11,14,
+17,40,44</t>
+  </si>
+  <si>
+    <t>1,4,8,11,14,
+17,40,43</t>
+  </si>
+  <si>
+    <t>1,4,8,11,13,
+21,25,29,33,40,44</t>
+  </si>
+  <si>
+    <t>1,4,8,11,13,
+21,25,29,33,40,43</t>
+  </si>
+  <si>
+    <t>1,4,8,12,14,
+17,40,46</t>
+  </si>
+  <si>
+    <t>1,4,8,11,15,
+21,25,29,33,40,43</t>
+  </si>
+  <si>
+    <t>1,4,8,11,14,
+17,42,43</t>
+  </si>
+  <si>
+    <t>1,4,8,11,13,
+17,21,25,31,33,40,43</t>
   </si>
 </sst>
 </file>
@@ -1074,7 +1151,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
@@ -1174,9 +1251,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -1209,6 +1283,48 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -2052,21 +2168,21 @@
   </sheetPr>
   <dimension ref="A1:AS73"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H14" sqref="H14"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X26" sqref="X26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="60" customWidth="1"/>
+    <col min="3" max="3" width="10" style="65" customWidth="1"/>
     <col min="4" max="4" width="99.85546875" style="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40.42578125" style="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="44.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="52" style="12" customWidth="1"/>
-    <col min="8" max="8" width="22" style="12" customWidth="1"/>
+    <col min="7" max="7" width="52" style="59" customWidth="1"/>
+    <col min="8" max="8" width="22" style="59" customWidth="1"/>
     <col min="9" max="9" width="9.85546875" style="2" customWidth="1"/>
     <col min="10" max="10" width="19.5703125" style="8" customWidth="1"/>
     <col min="11" max="11" width="13.7109375" style="24" customWidth="1"/>
@@ -2087,13 +2203,13 @@
   <sheetData>
     <row r="1" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A1" s="30"/>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="64"/>
       <c r="D1" s="31"/>
       <c r="E1" s="31"/>
       <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
       <c r="I1" s="31"/>
       <c r="J1" s="31"/>
       <c r="K1" s="31"/>
@@ -2119,16 +2235,16 @@
       <c r="AE1" s="4"/>
     </row>
     <row r="2" spans="1:45" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
       <c r="I2" s="32"/>
       <c r="J2" s="32"/>
       <c r="K2" s="32"/>
@@ -2154,14 +2270,14 @@
       <c r="AE2" s="4"/>
     </row>
     <row r="3" spans="1:45" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="48"/>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
+      <c r="A3" s="47"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
       <c r="I3" s="32"/>
       <c r="J3" s="32"/>
       <c r="K3" s="32"/>
@@ -2187,14 +2303,14 @@
       <c r="AE3" s="4"/>
     </row>
     <row r="4" spans="1:45" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="48"/>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
+      <c r="A4" s="47"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
       <c r="I4" s="32"/>
       <c r="J4" s="32"/>
       <c r="K4" s="32"/>
@@ -2220,16 +2336,16 @@
       <c r="AE4" s="4"/>
     </row>
     <row r="5" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="A5" s="50" t="s">
+      <c r="A5" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="50"/>
-      <c r="C5" s="43"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
       <c r="I5" s="33"/>
       <c r="J5" s="33"/>
       <c r="K5" s="33"/>
@@ -2254,8 +2370,8 @@
       <c r="AD5" s="4"/>
     </row>
     <row r="6" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="58"/>
       <c r="I6" s="4"/>
       <c r="J6" s="34"/>
       <c r="K6" s="35"/>
@@ -2281,34 +2397,34 @@
     </row>
     <row r="7" spans="1:45" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:45" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="51"/>
-      <c r="B8" s="51"/>
-      <c r="C8" s="51"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51"/>
-      <c r="G8" s="51"/>
-      <c r="H8" s="49" t="s">
+      <c r="A8" s="50"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="48" t="s">
         <v>76</v>
       </c>
-      <c r="I8" s="49"/>
-      <c r="J8" s="49"/>
-      <c r="K8" s="49"/>
-      <c r="L8" s="49"/>
-      <c r="M8" s="49" t="s">
+      <c r="I8" s="48"/>
+      <c r="J8" s="48"/>
+      <c r="K8" s="48"/>
+      <c r="L8" s="48"/>
+      <c r="M8" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="N8" s="49"/>
-      <c r="O8" s="49"/>
-      <c r="P8" s="49"/>
-      <c r="Q8" s="49"/>
-      <c r="R8" s="49" t="s">
+      <c r="N8" s="48"/>
+      <c r="O8" s="48"/>
+      <c r="P8" s="48"/>
+      <c r="Q8" s="48"/>
+      <c r="R8" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="S8" s="49"/>
-      <c r="T8" s="49"/>
-      <c r="U8" s="49"/>
-      <c r="V8" s="49"/>
+      <c r="S8" s="48"/>
+      <c r="T8" s="48"/>
+      <c r="U8" s="48"/>
+      <c r="V8" s="48"/>
     </row>
     <row r="9" spans="1:45" ht="24" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
@@ -2383,7 +2499,7 @@
     <row r="10" spans="1:45" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="17"/>
       <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
+      <c r="C10" s="66"/>
       <c r="D10" s="18"/>
       <c r="E10" s="19"/>
       <c r="F10" s="18"/>
@@ -2410,11 +2526,13 @@
       <c r="A11" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="61" t="s">
         <v>97</v>
       </c>
-      <c r="C11" s="26"/>
-      <c r="D11" s="47" t="s">
+      <c r="C11" s="67" t="s">
+        <v>161</v>
+      </c>
+      <c r="D11" s="46" t="s">
         <v>95</v>
       </c>
       <c r="E11" s="26" t="s">
@@ -2423,18 +2541,24 @@
       <c r="F11" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="G11" s="26" t="s">
-        <v>140</v>
-      </c>
-      <c r="H11" s="26" t="s">
+      <c r="G11" s="54" t="s">
+        <v>139</v>
+      </c>
+      <c r="H11" s="54" t="s">
         <v>88</v>
       </c>
       <c r="I11" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="J11" s="29"/>
-      <c r="K11" s="37"/>
-      <c r="L11" s="39"/>
+        <v>126</v>
+      </c>
+      <c r="J11" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="K11" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="L11" s="39" t="s">
+        <v>158</v>
+      </c>
       <c r="M11" s="15"/>
       <c r="N11" s="28"/>
       <c r="O11" s="29"/>
@@ -2456,11 +2580,13 @@
       <c r="A12" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="61" t="s">
         <v>97</v>
       </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="47" t="s">
+      <c r="C12" s="61" t="s">
+        <v>167</v>
+      </c>
+      <c r="D12" s="46" t="s">
         <v>96</v>
       </c>
       <c r="E12" s="26" t="s">
@@ -2469,18 +2595,24 @@
       <c r="F12" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="G12" s="26" t="s">
-        <v>140</v>
-      </c>
-      <c r="H12" s="26" t="s">
+      <c r="G12" s="54" t="s">
+        <v>139</v>
+      </c>
+      <c r="H12" s="54" t="s">
         <v>88</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="J12" s="28"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="37"/>
+        <v>126</v>
+      </c>
+      <c r="J12" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="K12" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="L12" s="37" t="s">
+        <v>158</v>
+      </c>
       <c r="M12" s="39"/>
       <c r="N12" s="15"/>
       <c r="O12" s="28"/>
@@ -2498,37 +2630,43 @@
       <c r="AR12" s="7"/>
       <c r="AS12" s="7"/>
     </row>
-    <row r="13" spans="1:45" ht="156" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:45" ht="144" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="61" t="s">
         <v>97</v>
       </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="47" t="s">
-        <v>103</v>
+      <c r="C13" s="61" t="s">
+        <v>166</v>
+      </c>
+      <c r="D13" s="46" t="s">
+        <v>102</v>
       </c>
       <c r="E13" s="26" t="s">
         <v>91</v>
       </c>
       <c r="F13" s="26" t="s">
-        <v>109</v>
-      </c>
-      <c r="G13" s="26" t="s">
-        <v>139</v>
-      </c>
-      <c r="H13" s="26" t="s">
-        <v>145</v>
+        <v>108</v>
+      </c>
+      <c r="G13" s="54" t="s">
+        <v>138</v>
+      </c>
+      <c r="H13" s="54" t="s">
+        <v>144</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="J13" s="28"/>
+        <v>125</v>
+      </c>
+      <c r="J13" s="29" t="s">
+        <v>159</v>
+      </c>
       <c r="K13" s="29">
         <v>1</v>
       </c>
-      <c r="L13" s="37"/>
+      <c r="L13" s="37" t="s">
+        <v>158</v>
+      </c>
       <c r="M13" s="39"/>
       <c r="N13" s="15"/>
       <c r="O13" s="28"/>
@@ -2546,37 +2684,43 @@
       <c r="AR13" s="7"/>
       <c r="AS13" s="7"/>
     </row>
-    <row r="14" spans="1:45" ht="156" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:45" ht="144" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="61" t="s">
         <v>97</v>
       </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="47" t="s">
-        <v>104</v>
+      <c r="C14" s="61" t="s">
+        <v>165</v>
+      </c>
+      <c r="D14" s="46" t="s">
+        <v>103</v>
       </c>
       <c r="E14" s="26" t="s">
         <v>91</v>
       </c>
       <c r="F14" s="26" t="s">
-        <v>110</v>
-      </c>
-      <c r="G14" s="26" t="s">
-        <v>139</v>
-      </c>
-      <c r="H14" s="26" t="s">
-        <v>146</v>
+        <v>109</v>
+      </c>
+      <c r="G14" s="54" t="s">
+        <v>138</v>
+      </c>
+      <c r="H14" s="54" t="s">
+        <v>145</v>
       </c>
       <c r="I14" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="J14" s="28"/>
+        <v>125</v>
+      </c>
+      <c r="J14" s="29" t="s">
+        <v>159</v>
+      </c>
       <c r="K14" s="29">
         <v>1</v>
       </c>
-      <c r="L14" s="37"/>
+      <c r="L14" s="37" t="s">
+        <v>158</v>
+      </c>
       <c r="M14" s="39"/>
       <c r="N14" s="15"/>
       <c r="O14" s="28"/>
@@ -2598,33 +2742,39 @@
       <c r="A15" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="61" t="s">
         <v>97</v>
       </c>
-      <c r="C15" s="21"/>
-      <c r="D15" s="47" t="s">
+      <c r="C15" s="67" t="s">
+        <v>168</v>
+      </c>
+      <c r="D15" s="46" t="s">
         <v>94</v>
       </c>
       <c r="E15" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="G15" s="54" t="s">
+        <v>140</v>
+      </c>
+      <c r="H15" s="54" t="s">
         <v>112</v>
       </c>
-      <c r="F15" s="26" t="s">
-        <v>114</v>
-      </c>
-      <c r="G15" s="26" t="s">
-        <v>141</v>
-      </c>
-      <c r="H15" s="26" t="s">
-        <v>113</v>
-      </c>
       <c r="I15" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="J15" s="28"/>
+        <v>125</v>
+      </c>
+      <c r="J15" s="29" t="s">
+        <v>159</v>
+      </c>
       <c r="K15" s="29">
         <v>1</v>
       </c>
-      <c r="L15" s="37"/>
+      <c r="L15" s="37" t="s">
+        <v>158</v>
+      </c>
       <c r="M15" s="39"/>
       <c r="N15" s="15"/>
       <c r="O15" s="28"/>
@@ -2646,33 +2796,39 @@
       <c r="A16" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="61" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="47" t="s">
-        <v>100</v>
+      <c r="C16" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="D16" s="46" t="s">
+        <v>162</v>
       </c>
       <c r="E16" s="26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F16" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="G16" s="26" t="s">
-        <v>142</v>
-      </c>
-      <c r="H16" s="26" t="s">
-        <v>113</v>
+        <v>114</v>
+      </c>
+      <c r="G16" s="54" t="s">
+        <v>141</v>
+      </c>
+      <c r="H16" s="54" t="s">
+        <v>112</v>
       </c>
       <c r="I16" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="J16" s="28"/>
+        <v>125</v>
+      </c>
+      <c r="J16" s="29" t="s">
+        <v>159</v>
+      </c>
       <c r="K16" s="29">
         <v>2</v>
       </c>
-      <c r="L16" s="37"/>
+      <c r="L16" s="37" t="s">
+        <v>158</v>
+      </c>
       <c r="M16" s="39"/>
       <c r="N16" s="15"/>
       <c r="O16" s="28"/>
@@ -2690,35 +2846,43 @@
       <c r="AR16" s="7"/>
       <c r="AS16" s="7"/>
     </row>
-    <row r="17" spans="1:45" ht="108" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:45" ht="96" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="61" t="s">
         <v>97</v>
       </c>
-      <c r="C17" s="21"/>
-      <c r="D17" s="47" t="s">
+      <c r="C17" s="67" t="s">
+        <v>164</v>
+      </c>
+      <c r="D17" s="46" t="s">
+        <v>117</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="F17" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="E17" s="26" t="s">
-        <v>111</v>
-      </c>
-      <c r="F17" s="26" t="s">
+      <c r="G17" s="54" t="s">
+        <v>141</v>
+      </c>
+      <c r="H17" s="54" t="s">
         <v>119</v>
       </c>
-      <c r="G17" s="26" t="s">
-        <v>142</v>
-      </c>
-      <c r="H17" s="26" t="s">
-        <v>120</v>
-      </c>
       <c r="I17" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="J17" s="28"/>
-      <c r="K17" s="29"/>
-      <c r="L17" s="37"/>
+        <v>126</v>
+      </c>
+      <c r="J17" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="K17" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="L17" s="37" t="s">
+        <v>158</v>
+      </c>
       <c r="M17" s="39"/>
       <c r="N17" s="15"/>
       <c r="O17" s="28"/>
@@ -2740,31 +2904,39 @@
       <c r="A18" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="61" t="s">
         <v>97</v>
       </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="47" t="s">
-        <v>101</v>
+      <c r="C18" s="67" t="s">
+        <v>169</v>
+      </c>
+      <c r="D18" s="46" t="s">
+        <v>100</v>
       </c>
       <c r="E18" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="F18" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="F18" s="26" t="s">
-        <v>117</v>
-      </c>
-      <c r="G18" s="26" t="s">
-        <v>141</v>
-      </c>
-      <c r="H18" s="26" t="s">
-        <v>144</v>
+      <c r="G18" s="54" t="s">
+        <v>140</v>
+      </c>
+      <c r="H18" s="54" t="s">
+        <v>143</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="J18" s="28"/>
-      <c r="K18" s="29"/>
-      <c r="L18" s="37"/>
+        <v>126</v>
+      </c>
+      <c r="J18" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="K18" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="L18" s="37" t="s">
+        <v>158</v>
+      </c>
       <c r="M18" s="39"/>
       <c r="N18" s="15"/>
       <c r="O18" s="28"/>
@@ -2786,31 +2958,39 @@
       <c r="A19" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="61" t="s">
         <v>97</v>
       </c>
-      <c r="C19" s="21"/>
-      <c r="D19" s="47" t="s">
-        <v>102</v>
+      <c r="C19" s="67" t="s">
+        <v>170</v>
+      </c>
+      <c r="D19" s="46" t="s">
+        <v>101</v>
       </c>
       <c r="E19" s="26" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F19" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="G19" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="G19" s="54" t="s">
+        <v>142</v>
+      </c>
+      <c r="H19" s="54" t="s">
         <v>143</v>
       </c>
-      <c r="H19" s="26" t="s">
-        <v>144</v>
-      </c>
       <c r="I19" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="J19" s="28"/>
-      <c r="K19" s="29"/>
-      <c r="L19" s="37"/>
+        <v>126</v>
+      </c>
+      <c r="J19" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="K19" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="L19" s="37" t="s">
+        <v>158</v>
+      </c>
       <c r="M19" s="39"/>
       <c r="N19" s="15"/>
       <c r="O19" s="28"/>
@@ -2832,11 +3012,13 @@
       <c r="A20" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="61" t="s">
         <v>97</v>
       </c>
-      <c r="C20" s="26"/>
-      <c r="D20" s="47" t="s">
+      <c r="C20" s="67" t="s">
+        <v>171</v>
+      </c>
+      <c r="D20" s="46" t="s">
         <v>98</v>
       </c>
       <c r="E20" s="26" t="s">
@@ -2845,18 +3027,24 @@
       <c r="F20" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="G20" s="26" t="s">
-        <v>140</v>
-      </c>
-      <c r="H20" s="26" t="s">
+      <c r="G20" s="54" t="s">
+        <v>139</v>
+      </c>
+      <c r="H20" s="54" t="s">
         <v>88</v>
       </c>
       <c r="I20" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="J20" s="28"/>
-      <c r="K20" s="29"/>
-      <c r="L20" s="37"/>
+        <v>126</v>
+      </c>
+      <c r="J20" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="K20" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="L20" s="37" t="s">
+        <v>158</v>
+      </c>
       <c r="M20" s="39"/>
       <c r="N20" s="15"/>
       <c r="O20" s="28"/>
@@ -2878,31 +3066,39 @@
       <c r="A21" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="21" t="s">
+      <c r="B21" s="61" t="s">
         <v>97</v>
       </c>
-      <c r="C21" s="21"/>
-      <c r="D21" s="47" t="s">
-        <v>105</v>
+      <c r="C21" s="67" t="s">
+        <v>172</v>
+      </c>
+      <c r="D21" s="46" t="s">
+        <v>104</v>
       </c>
       <c r="E21" s="26" t="s">
         <v>89</v>
       </c>
       <c r="F21" s="26" t="s">
-        <v>108</v>
-      </c>
-      <c r="G21" s="26" t="s">
-        <v>140</v>
-      </c>
-      <c r="H21" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="G21" s="54" t="s">
+        <v>139</v>
+      </c>
+      <c r="H21" s="54" t="s">
         <v>88</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="J21" s="28"/>
-      <c r="K21" s="29"/>
-      <c r="L21" s="37"/>
+        <v>126</v>
+      </c>
+      <c r="J21" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="K21" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="L21" s="37" t="s">
+        <v>158</v>
+      </c>
       <c r="M21" s="39"/>
       <c r="N21" s="15"/>
       <c r="O21" s="28"/>
@@ -2920,16 +3116,18 @@
       <c r="AR21" s="7"/>
       <c r="AS21" s="7"/>
     </row>
-    <row r="22" spans="1:45" ht="156" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:45" ht="144" x14ac:dyDescent="0.2">
       <c r="A22" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="61" t="s">
         <v>97</v>
       </c>
-      <c r="C22" s="21"/>
-      <c r="D22" s="47" t="s">
-        <v>106</v>
+      <c r="C22" s="61" t="s">
+        <v>173</v>
+      </c>
+      <c r="D22" s="46" t="s">
+        <v>105</v>
       </c>
       <c r="E22" s="26" t="s">
         <v>91</v>
@@ -2937,20 +3135,24 @@
       <c r="F22" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="G22" s="26" t="s">
-        <v>139</v>
-      </c>
-      <c r="H22" s="26" t="s">
-        <v>146</v>
+      <c r="G22" s="54" t="s">
+        <v>138</v>
+      </c>
+      <c r="H22" s="54" t="s">
+        <v>145</v>
       </c>
       <c r="I22" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="J22" s="28"/>
+        <v>125</v>
+      </c>
+      <c r="J22" s="29" t="s">
+        <v>159</v>
+      </c>
       <c r="K22" s="29">
         <v>1</v>
       </c>
-      <c r="L22" s="37"/>
+      <c r="L22" s="37" t="s">
+        <v>158</v>
+      </c>
       <c r="M22" s="39"/>
       <c r="N22" s="15"/>
       <c r="O22" s="28"/>
@@ -2968,16 +3170,18 @@
       <c r="AR22" s="7"/>
       <c r="AS22" s="7"/>
     </row>
-    <row r="23" spans="1:45" ht="156" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:45" ht="144" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="61" t="s">
         <v>97</v>
       </c>
-      <c r="C23" s="21"/>
-      <c r="D23" s="47" t="s">
-        <v>107</v>
+      <c r="C23" s="61" t="s">
+        <v>174</v>
+      </c>
+      <c r="D23" s="46" t="s">
+        <v>106</v>
       </c>
       <c r="E23" s="26" t="s">
         <v>91</v>
@@ -2985,18 +3189,24 @@
       <c r="F23" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="G23" s="26" t="s">
-        <v>139</v>
-      </c>
-      <c r="H23" s="26" t="s">
-        <v>146</v>
+      <c r="G23" s="54" t="s">
+        <v>138</v>
+      </c>
+      <c r="H23" s="54" t="s">
+        <v>145</v>
       </c>
       <c r="I23" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="J23" s="28"/>
-      <c r="K23" s="29"/>
-      <c r="L23" s="37"/>
+        <v>126</v>
+      </c>
+      <c r="J23" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="K23" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="L23" s="37" t="s">
+        <v>158</v>
+      </c>
       <c r="M23" s="39"/>
       <c r="N23" s="15"/>
       <c r="O23" s="28"/>
@@ -3018,33 +3228,39 @@
       <c r="A24" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="61" t="s">
         <v>97</v>
       </c>
-      <c r="C24" s="26"/>
-      <c r="D24" s="47" t="s">
-        <v>122</v>
+      <c r="C24" s="67" t="s">
+        <v>175</v>
+      </c>
+      <c r="D24" s="46" t="s">
+        <v>121</v>
       </c>
       <c r="E24" s="26" t="s">
         <v>86</v>
       </c>
       <c r="F24" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="G24" s="54" t="s">
         <v>123</v>
       </c>
-      <c r="G24" s="26" t="s">
+      <c r="H24" s="54" t="s">
         <v>124</v>
       </c>
-      <c r="H24" s="26" t="s">
+      <c r="I24" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="I24" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="J24" s="28"/>
+      <c r="J24" s="29" t="s">
+        <v>159</v>
+      </c>
       <c r="K24" s="29">
         <v>3</v>
       </c>
-      <c r="L24" s="37"/>
+      <c r="L24" s="37" t="s">
+        <v>158</v>
+      </c>
       <c r="M24" s="39"/>
       <c r="N24" s="15"/>
       <c r="O24" s="28"/>
@@ -3062,35 +3278,43 @@
       <c r="AR24" s="7"/>
       <c r="AS24" s="7"/>
     </row>
-    <row r="25" spans="1:45" ht="156" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:45" ht="144" x14ac:dyDescent="0.2">
       <c r="A25" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="61" t="s">
         <v>97</v>
       </c>
-      <c r="C25" s="21"/>
-      <c r="D25" s="47" t="s">
+      <c r="C25" s="61" t="s">
+        <v>176</v>
+      </c>
+      <c r="D25" s="46" t="s">
+        <v>127</v>
+      </c>
+      <c r="E25" s="26" t="s">
         <v>128</v>
-      </c>
-      <c r="E25" s="26" t="s">
-        <v>129</v>
       </c>
       <c r="F25" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="G25" s="26" t="s">
-        <v>138</v>
-      </c>
-      <c r="H25" s="26" t="s">
-        <v>130</v>
+      <c r="G25" s="54" t="s">
+        <v>137</v>
+      </c>
+      <c r="H25" s="54" t="s">
+        <v>129</v>
       </c>
       <c r="I25" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="J25" s="28"/>
-      <c r="K25" s="29"/>
-      <c r="L25" s="37"/>
+        <v>126</v>
+      </c>
+      <c r="J25" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="K25" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="L25" s="37" t="s">
+        <v>158</v>
+      </c>
       <c r="M25" s="39"/>
       <c r="N25" s="15"/>
       <c r="O25" s="28"/>
@@ -3112,33 +3336,39 @@
       <c r="A26" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="61" t="s">
         <v>97</v>
       </c>
-      <c r="C26" s="21"/>
-      <c r="D26" s="47" t="s">
+      <c r="C26" s="61" t="s">
+        <v>178</v>
+      </c>
+      <c r="D26" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="E26" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="E26" s="26" t="s">
+      <c r="F26" s="44" t="s">
         <v>132</v>
       </c>
-      <c r="F26" s="45" t="s">
-        <v>133</v>
-      </c>
-      <c r="G26" s="26" t="s">
-        <v>138</v>
-      </c>
-      <c r="H26" s="26" t="s">
-        <v>147</v>
+      <c r="G26" s="54" t="s">
+        <v>137</v>
+      </c>
+      <c r="H26" s="54" t="s">
+        <v>146</v>
       </c>
       <c r="I26" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="J26" s="28"/>
+        <v>125</v>
+      </c>
+      <c r="J26" s="29" t="s">
+        <v>159</v>
+      </c>
       <c r="K26" s="29">
         <v>5</v>
       </c>
-      <c r="L26" s="37"/>
+      <c r="L26" s="37" t="s">
+        <v>158</v>
+      </c>
       <c r="M26" s="39"/>
       <c r="N26" s="15"/>
       <c r="O26" s="28"/>
@@ -3156,35 +3386,43 @@
       <c r="AR26" s="7"/>
       <c r="AS26" s="7"/>
     </row>
-    <row r="27" spans="1:45" ht="96" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:45" ht="84" x14ac:dyDescent="0.2">
       <c r="A27" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="21" t="s">
+      <c r="B27" s="61" t="s">
         <v>97</v>
       </c>
-      <c r="C27" s="21"/>
-      <c r="D27" s="47" t="s">
+      <c r="C27" s="61" t="s">
+        <v>177</v>
+      </c>
+      <c r="D27" s="46" t="s">
+        <v>133</v>
+      </c>
+      <c r="E27" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="E27" s="26" t="s">
+      <c r="F27" s="45" t="s">
         <v>135</v>
       </c>
-      <c r="F27" s="46" t="s">
+      <c r="G27" s="54" t="s">
         <v>136</v>
       </c>
-      <c r="G27" s="26" t="s">
-        <v>137</v>
-      </c>
-      <c r="H27" s="26" t="s">
-        <v>137</v>
+      <c r="H27" s="54" t="s">
+        <v>136</v>
       </c>
       <c r="I27" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="J27" s="28"/>
-      <c r="K27" s="29"/>
-      <c r="L27" s="37"/>
+        <v>126</v>
+      </c>
+      <c r="J27" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="K27" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="L27" s="37" t="s">
+        <v>158</v>
+      </c>
       <c r="M27" s="39"/>
       <c r="N27" s="15"/>
       <c r="O27" s="28"/>
@@ -3206,13 +3444,13 @@
       <c r="A28" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
+      <c r="B28" s="61"/>
+      <c r="C28" s="61"/>
       <c r="D28" s="21"/>
       <c r="E28" s="26"/>
       <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="26"/>
+      <c r="G28" s="54"/>
+      <c r="H28" s="54"/>
       <c r="I28" s="15"/>
       <c r="J28" s="28"/>
       <c r="K28" s="29"/>
@@ -3238,13 +3476,13 @@
       <c r="A29" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
+      <c r="B29" s="61"/>
+      <c r="C29" s="61"/>
       <c r="D29" s="21"/>
       <c r="E29" s="26"/>
       <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
+      <c r="G29" s="54"/>
+      <c r="H29" s="54"/>
       <c r="I29" s="15"/>
       <c r="J29" s="28"/>
       <c r="K29" s="29"/>
@@ -3270,13 +3508,13 @@
       <c r="A30" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B30" s="21"/>
-      <c r="C30" s="21"/>
+      <c r="B30" s="61"/>
+      <c r="C30" s="61"/>
       <c r="D30" s="21"/>
       <c r="E30" s="26"/>
       <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
+      <c r="G30" s="54"/>
+      <c r="H30" s="54"/>
       <c r="I30" s="15"/>
       <c r="J30" s="28"/>
       <c r="K30" s="29"/>
@@ -3302,13 +3540,13 @@
       <c r="A31" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
+      <c r="B31" s="61"/>
+      <c r="C31" s="61"/>
       <c r="D31" s="21"/>
       <c r="E31" s="26"/>
       <c r="F31" s="26"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="26"/>
+      <c r="G31" s="54"/>
+      <c r="H31" s="54"/>
       <c r="I31" s="15"/>
       <c r="J31" s="28"/>
       <c r="K31" s="29"/>
@@ -3334,13 +3572,13 @@
       <c r="A32" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="B32" s="21"/>
-      <c r="C32" s="21"/>
+      <c r="B32" s="61"/>
+      <c r="C32" s="61"/>
       <c r="D32" s="21"/>
       <c r="E32" s="26"/>
       <c r="F32" s="26"/>
-      <c r="G32" s="26"/>
-      <c r="H32" s="26"/>
+      <c r="G32" s="54"/>
+      <c r="H32" s="54"/>
       <c r="I32" s="15"/>
       <c r="J32" s="28"/>
       <c r="K32" s="29"/>
@@ -3366,13 +3604,13 @@
       <c r="A33" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
+      <c r="B33" s="61"/>
+      <c r="C33" s="61"/>
       <c r="D33" s="21"/>
       <c r="E33" s="26"/>
       <c r="F33" s="26"/>
-      <c r="G33" s="26"/>
-      <c r="H33" s="26"/>
+      <c r="G33" s="54"/>
+      <c r="H33" s="54"/>
       <c r="I33" s="15"/>
       <c r="J33" s="28"/>
       <c r="K33" s="29"/>
@@ -3398,13 +3636,13 @@
       <c r="A34" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="B34" s="21"/>
-      <c r="C34" s="21"/>
+      <c r="B34" s="61"/>
+      <c r="C34" s="61"/>
       <c r="D34" s="21"/>
       <c r="E34" s="26"/>
       <c r="F34" s="26"/>
-      <c r="G34" s="26"/>
-      <c r="H34" s="26"/>
+      <c r="G34" s="54"/>
+      <c r="H34" s="54"/>
       <c r="I34" s="15"/>
       <c r="J34" s="28"/>
       <c r="K34" s="29"/>
@@ -3430,13 +3668,13 @@
       <c r="A35" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
+      <c r="B35" s="61"/>
+      <c r="C35" s="61"/>
       <c r="D35" s="21"/>
       <c r="E35" s="26"/>
       <c r="F35" s="26"/>
-      <c r="G35" s="26"/>
-      <c r="H35" s="26"/>
+      <c r="G35" s="54"/>
+      <c r="H35" s="54"/>
       <c r="I35" s="15"/>
       <c r="J35" s="28"/>
       <c r="K35" s="29"/>
@@ -3462,13 +3700,13 @@
       <c r="A36" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="21"/>
-      <c r="C36" s="21"/>
+      <c r="B36" s="61"/>
+      <c r="C36" s="61"/>
       <c r="D36" s="21"/>
       <c r="E36" s="26"/>
       <c r="F36" s="26"/>
-      <c r="G36" s="26"/>
-      <c r="H36" s="26"/>
+      <c r="G36" s="54"/>
+      <c r="H36" s="54"/>
       <c r="I36" s="15"/>
       <c r="J36" s="28"/>
       <c r="K36" s="29"/>
@@ -3494,13 +3732,13 @@
       <c r="A37" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
+      <c r="B37" s="61"/>
+      <c r="C37" s="61"/>
       <c r="D37" s="21"/>
       <c r="E37" s="26"/>
       <c r="F37" s="26"/>
-      <c r="G37" s="26"/>
-      <c r="H37" s="26"/>
+      <c r="G37" s="54"/>
+      <c r="H37" s="54"/>
       <c r="I37" s="15"/>
       <c r="J37" s="28"/>
       <c r="K37" s="29"/>
@@ -3526,13 +3764,13 @@
       <c r="A38" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B38" s="21"/>
-      <c r="C38" s="21"/>
+      <c r="B38" s="61"/>
+      <c r="C38" s="61"/>
       <c r="D38" s="21"/>
       <c r="E38" s="26"/>
       <c r="F38" s="26"/>
-      <c r="G38" s="26"/>
-      <c r="H38" s="26"/>
+      <c r="G38" s="54"/>
+      <c r="H38" s="54"/>
       <c r="I38" s="15"/>
       <c r="J38" s="28"/>
       <c r="K38" s="29"/>
@@ -3558,13 +3796,13 @@
       <c r="A39" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B39" s="21"/>
-      <c r="C39" s="21"/>
+      <c r="B39" s="61"/>
+      <c r="C39" s="61"/>
       <c r="D39" s="21"/>
       <c r="E39" s="26"/>
       <c r="F39" s="26"/>
-      <c r="G39" s="26"/>
-      <c r="H39" s="26"/>
+      <c r="G39" s="54"/>
+      <c r="H39" s="54"/>
       <c r="I39" s="15"/>
       <c r="J39" s="28"/>
       <c r="K39" s="29"/>
@@ -3590,13 +3828,13 @@
       <c r="A40" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B40" s="21"/>
-      <c r="C40" s="21"/>
+      <c r="B40" s="61"/>
+      <c r="C40" s="61"/>
       <c r="D40" s="21"/>
       <c r="E40" s="26"/>
       <c r="F40" s="26"/>
-      <c r="G40" s="26"/>
-      <c r="H40" s="26"/>
+      <c r="G40" s="54"/>
+      <c r="H40" s="54"/>
       <c r="I40" s="15"/>
       <c r="J40" s="28"/>
       <c r="K40" s="29"/>
@@ -3622,13 +3860,13 @@
       <c r="A41" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B41" s="21"/>
-      <c r="C41" s="21"/>
+      <c r="B41" s="61"/>
+      <c r="C41" s="61"/>
       <c r="D41" s="21"/>
       <c r="E41" s="26"/>
       <c r="F41" s="26"/>
-      <c r="G41" s="26"/>
-      <c r="H41" s="26"/>
+      <c r="G41" s="54"/>
+      <c r="H41" s="54"/>
       <c r="I41" s="15"/>
       <c r="J41" s="28"/>
       <c r="K41" s="29"/>
@@ -3654,13 +3892,13 @@
       <c r="A42" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B42" s="21"/>
-      <c r="C42" s="21"/>
+      <c r="B42" s="61"/>
+      <c r="C42" s="61"/>
       <c r="D42" s="21"/>
       <c r="E42" s="26"/>
       <c r="F42" s="26"/>
-      <c r="G42" s="26"/>
-      <c r="H42" s="26"/>
+      <c r="G42" s="54"/>
+      <c r="H42" s="54"/>
       <c r="I42" s="15"/>
       <c r="J42" s="28"/>
       <c r="K42" s="29"/>
@@ -3686,13 +3924,13 @@
       <c r="A43" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B43" s="21"/>
-      <c r="C43" s="21"/>
+      <c r="B43" s="61"/>
+      <c r="C43" s="61"/>
       <c r="D43" s="21"/>
       <c r="E43" s="26"/>
       <c r="F43" s="26"/>
-      <c r="G43" s="26"/>
-      <c r="H43" s="26"/>
+      <c r="G43" s="54"/>
+      <c r="H43" s="54"/>
       <c r="I43" s="15"/>
       <c r="J43" s="28"/>
       <c r="K43" s="29"/>
@@ -3718,13 +3956,13 @@
       <c r="A44" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B44" s="21"/>
-      <c r="C44" s="21"/>
+      <c r="B44" s="61"/>
+      <c r="C44" s="61"/>
       <c r="D44" s="21"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
-      <c r="G44" s="26"/>
-      <c r="H44" s="26"/>
+      <c r="G44" s="54"/>
+      <c r="H44" s="54"/>
       <c r="I44" s="15"/>
       <c r="J44" s="28"/>
       <c r="K44" s="29"/>
@@ -3750,13 +3988,13 @@
       <c r="A45" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B45" s="21"/>
-      <c r="C45" s="21"/>
+      <c r="B45" s="61"/>
+      <c r="C45" s="61"/>
       <c r="D45" s="21"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
-      <c r="G45" s="26"/>
-      <c r="H45" s="26"/>
+      <c r="G45" s="54"/>
+      <c r="H45" s="54"/>
       <c r="I45" s="15"/>
       <c r="J45" s="28"/>
       <c r="K45" s="29"/>
@@ -3782,13 +4020,13 @@
       <c r="A46" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B46" s="21"/>
-      <c r="C46" s="21"/>
+      <c r="B46" s="61"/>
+      <c r="C46" s="61"/>
       <c r="D46" s="21"/>
       <c r="E46" s="26"/>
       <c r="F46" s="26"/>
-      <c r="G46" s="26"/>
-      <c r="H46" s="26"/>
+      <c r="G46" s="54"/>
+      <c r="H46" s="54"/>
       <c r="I46" s="15"/>
       <c r="J46" s="28"/>
       <c r="K46" s="29"/>
@@ -3814,13 +4052,13 @@
       <c r="A47" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B47" s="21"/>
-      <c r="C47" s="21"/>
+      <c r="B47" s="61"/>
+      <c r="C47" s="61"/>
       <c r="D47" s="21"/>
       <c r="E47" s="26"/>
       <c r="F47" s="26"/>
-      <c r="G47" s="26"/>
-      <c r="H47" s="26"/>
+      <c r="G47" s="54"/>
+      <c r="H47" s="54"/>
       <c r="I47" s="15"/>
       <c r="J47" s="28"/>
       <c r="K47" s="29"/>
@@ -3846,13 +4084,13 @@
       <c r="A48" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B48" s="21"/>
-      <c r="C48" s="21"/>
+      <c r="B48" s="61"/>
+      <c r="C48" s="61"/>
       <c r="D48" s="21"/>
       <c r="E48" s="26"/>
       <c r="F48" s="26"/>
-      <c r="G48" s="26"/>
-      <c r="H48" s="26"/>
+      <c r="G48" s="54"/>
+      <c r="H48" s="54"/>
       <c r="I48" s="15"/>
       <c r="J48" s="28"/>
       <c r="K48" s="29"/>
@@ -3878,13 +4116,13 @@
       <c r="A49" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B49" s="21"/>
-      <c r="C49" s="21"/>
+      <c r="B49" s="61"/>
+      <c r="C49" s="61"/>
       <c r="D49" s="21"/>
       <c r="E49" s="26"/>
       <c r="F49" s="26"/>
-      <c r="G49" s="26"/>
-      <c r="H49" s="26"/>
+      <c r="G49" s="54"/>
+      <c r="H49" s="54"/>
       <c r="I49" s="15"/>
       <c r="J49" s="28"/>
       <c r="K49" s="29"/>
@@ -3910,13 +4148,13 @@
       <c r="A50" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B50" s="21"/>
-      <c r="C50" s="21"/>
+      <c r="B50" s="61"/>
+      <c r="C50" s="61"/>
       <c r="D50" s="21"/>
       <c r="E50" s="26"/>
       <c r="F50" s="26"/>
-      <c r="G50" s="26"/>
-      <c r="H50" s="26"/>
+      <c r="G50" s="54"/>
+      <c r="H50" s="54"/>
       <c r="I50" s="15"/>
       <c r="J50" s="28"/>
       <c r="K50" s="29"/>
@@ -3942,13 +4180,13 @@
       <c r="A51" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B51" s="21"/>
-      <c r="C51" s="21"/>
+      <c r="B51" s="61"/>
+      <c r="C51" s="61"/>
       <c r="D51" s="21"/>
       <c r="E51" s="26"/>
       <c r="F51" s="26"/>
-      <c r="G51" s="26"/>
-      <c r="H51" s="26"/>
+      <c r="G51" s="54"/>
+      <c r="H51" s="54"/>
       <c r="I51" s="15"/>
       <c r="J51" s="28"/>
       <c r="K51" s="29"/>
@@ -3974,13 +4212,13 @@
       <c r="A52" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B52" s="21"/>
-      <c r="C52" s="21"/>
+      <c r="B52" s="61"/>
+      <c r="C52" s="61"/>
       <c r="D52" s="21"/>
       <c r="E52" s="26"/>
       <c r="F52" s="26"/>
-      <c r="G52" s="26"/>
-      <c r="H52" s="26"/>
+      <c r="G52" s="54"/>
+      <c r="H52" s="54"/>
       <c r="I52" s="15"/>
       <c r="J52" s="28"/>
       <c r="K52" s="29"/>
@@ -4006,13 +4244,13 @@
       <c r="A53" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B53" s="21"/>
-      <c r="C53" s="21"/>
+      <c r="B53" s="61"/>
+      <c r="C53" s="61"/>
       <c r="D53" s="21"/>
       <c r="E53" s="26"/>
       <c r="F53" s="26"/>
-      <c r="G53" s="26"/>
-      <c r="H53" s="26"/>
+      <c r="G53" s="54"/>
+      <c r="H53" s="54"/>
       <c r="I53" s="15"/>
       <c r="J53" s="28"/>
       <c r="K53" s="29"/>
@@ -4038,13 +4276,13 @@
       <c r="A54" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B54" s="21"/>
-      <c r="C54" s="21"/>
+      <c r="B54" s="61"/>
+      <c r="C54" s="61"/>
       <c r="D54" s="21"/>
       <c r="E54" s="26"/>
       <c r="F54" s="26"/>
-      <c r="G54" s="26"/>
-      <c r="H54" s="26"/>
+      <c r="G54" s="54"/>
+      <c r="H54" s="54"/>
       <c r="I54" s="15"/>
       <c r="J54" s="28"/>
       <c r="K54" s="29"/>
@@ -4070,13 +4308,13 @@
       <c r="A55" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B55" s="21"/>
-      <c r="C55" s="21"/>
+      <c r="B55" s="61"/>
+      <c r="C55" s="61"/>
       <c r="D55" s="21"/>
       <c r="E55" s="26"/>
       <c r="F55" s="26"/>
-      <c r="G55" s="26"/>
-      <c r="H55" s="26"/>
+      <c r="G55" s="54"/>
+      <c r="H55" s="54"/>
       <c r="I55" s="15"/>
       <c r="J55" s="28"/>
       <c r="K55" s="29"/>
@@ -4102,13 +4340,13 @@
       <c r="A56" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B56" s="21"/>
-      <c r="C56" s="21"/>
+      <c r="B56" s="61"/>
+      <c r="C56" s="61"/>
       <c r="D56" s="21"/>
       <c r="E56" s="26"/>
       <c r="F56" s="26"/>
-      <c r="G56" s="26"/>
-      <c r="H56" s="26"/>
+      <c r="G56" s="54"/>
+      <c r="H56" s="54"/>
       <c r="I56" s="15"/>
       <c r="J56" s="28"/>
       <c r="K56" s="29"/>
@@ -4134,13 +4372,13 @@
       <c r="A57" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B57" s="21"/>
-      <c r="C57" s="21"/>
+      <c r="B57" s="61"/>
+      <c r="C57" s="61"/>
       <c r="D57" s="21"/>
       <c r="E57" s="26"/>
       <c r="F57" s="26"/>
-      <c r="G57" s="26"/>
-      <c r="H57" s="26"/>
+      <c r="G57" s="54"/>
+      <c r="H57" s="54"/>
       <c r="I57" s="15"/>
       <c r="J57" s="28"/>
       <c r="K57" s="29"/>
@@ -4166,13 +4404,13 @@
       <c r="A58" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B58" s="21"/>
-      <c r="C58" s="21"/>
+      <c r="B58" s="61"/>
+      <c r="C58" s="61"/>
       <c r="D58" s="21"/>
       <c r="E58" s="26"/>
       <c r="F58" s="26"/>
-      <c r="G58" s="26"/>
-      <c r="H58" s="26"/>
+      <c r="G58" s="54"/>
+      <c r="H58" s="54"/>
       <c r="I58" s="15"/>
       <c r="J58" s="28"/>
       <c r="K58" s="29"/>
@@ -4198,13 +4436,13 @@
       <c r="A59" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="B59" s="21"/>
-      <c r="C59" s="21"/>
+      <c r="B59" s="61"/>
+      <c r="C59" s="61"/>
       <c r="D59" s="21"/>
       <c r="E59" s="26"/>
       <c r="F59" s="26"/>
-      <c r="G59" s="26"/>
-      <c r="H59" s="26"/>
+      <c r="G59" s="54"/>
+      <c r="H59" s="54"/>
       <c r="I59" s="15"/>
       <c r="J59" s="28"/>
       <c r="K59" s="29"/>
@@ -4230,13 +4468,13 @@
       <c r="A60" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B60" s="21"/>
-      <c r="C60" s="21"/>
+      <c r="B60" s="61"/>
+      <c r="C60" s="61"/>
       <c r="D60" s="21"/>
       <c r="E60" s="26"/>
       <c r="F60" s="26"/>
-      <c r="G60" s="26"/>
-      <c r="H60" s="26"/>
+      <c r="G60" s="54"/>
+      <c r="H60" s="54"/>
       <c r="I60" s="15"/>
       <c r="J60" s="28"/>
       <c r="K60" s="29"/>
@@ -4262,13 +4500,13 @@
       <c r="A61" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B61" s="21"/>
-      <c r="C61" s="21"/>
+      <c r="B61" s="61"/>
+      <c r="C61" s="61"/>
       <c r="D61" s="21"/>
       <c r="E61" s="26"/>
       <c r="F61" s="26"/>
-      <c r="G61" s="26"/>
-      <c r="H61" s="26"/>
+      <c r="G61" s="54"/>
+      <c r="H61" s="54"/>
       <c r="I61" s="15"/>
       <c r="J61" s="28"/>
       <c r="K61" s="29"/>
@@ -4294,13 +4532,13 @@
       <c r="A62" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B62" s="21"/>
-      <c r="C62" s="21"/>
+      <c r="B62" s="61"/>
+      <c r="C62" s="61"/>
       <c r="D62" s="21"/>
       <c r="E62" s="26"/>
       <c r="F62" s="26"/>
-      <c r="G62" s="26"/>
-      <c r="H62" s="26"/>
+      <c r="G62" s="54"/>
+      <c r="H62" s="54"/>
       <c r="I62" s="15"/>
       <c r="J62" s="28"/>
       <c r="K62" s="29"/>
@@ -4326,13 +4564,13 @@
       <c r="A63" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B63" s="21"/>
-      <c r="C63" s="21"/>
+      <c r="B63" s="61"/>
+      <c r="C63" s="61"/>
       <c r="D63" s="21"/>
       <c r="E63" s="26"/>
       <c r="F63" s="26"/>
-      <c r="G63" s="26"/>
-      <c r="H63" s="26"/>
+      <c r="G63" s="54"/>
+      <c r="H63" s="54"/>
       <c r="I63" s="15"/>
       <c r="J63" s="28"/>
       <c r="K63" s="29"/>
@@ -4358,13 +4596,13 @@
       <c r="A64" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B64" s="21"/>
-      <c r="C64" s="21"/>
+      <c r="B64" s="61"/>
+      <c r="C64" s="61"/>
       <c r="D64" s="21"/>
       <c r="E64" s="26"/>
       <c r="F64" s="26"/>
-      <c r="G64" s="26"/>
-      <c r="H64" s="26"/>
+      <c r="G64" s="54"/>
+      <c r="H64" s="54"/>
       <c r="I64" s="15"/>
       <c r="J64" s="28"/>
       <c r="K64" s="29"/>
@@ -4390,13 +4628,13 @@
       <c r="A65" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B65" s="21"/>
-      <c r="C65" s="21"/>
+      <c r="B65" s="61"/>
+      <c r="C65" s="61"/>
       <c r="D65" s="21"/>
       <c r="E65" s="26"/>
       <c r="F65" s="26"/>
-      <c r="G65" s="26"/>
-      <c r="H65" s="26"/>
+      <c r="G65" s="54"/>
+      <c r="H65" s="54"/>
       <c r="I65" s="15"/>
       <c r="J65" s="28"/>
       <c r="K65" s="29"/>
@@ -4422,13 +4660,13 @@
       <c r="A66" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B66" s="21"/>
-      <c r="C66" s="21"/>
+      <c r="B66" s="61"/>
+      <c r="C66" s="61"/>
       <c r="D66" s="21"/>
       <c r="E66" s="26"/>
       <c r="F66" s="26"/>
-      <c r="G66" s="26"/>
-      <c r="H66" s="26"/>
+      <c r="G66" s="54"/>
+      <c r="H66" s="54"/>
       <c r="I66" s="15"/>
       <c r="J66" s="28"/>
       <c r="K66" s="29"/>
@@ -4454,13 +4692,13 @@
       <c r="A67" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="B67" s="21"/>
-      <c r="C67" s="21"/>
+      <c r="B67" s="61"/>
+      <c r="C67" s="61"/>
       <c r="D67" s="21"/>
       <c r="E67" s="26"/>
       <c r="F67" s="26"/>
-      <c r="G67" s="26"/>
-      <c r="H67" s="26"/>
+      <c r="G67" s="54"/>
+      <c r="H67" s="54"/>
       <c r="I67" s="15"/>
       <c r="J67" s="28"/>
       <c r="K67" s="29"/>
@@ -4486,13 +4724,13 @@
       <c r="A68" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B68" s="21"/>
-      <c r="C68" s="21"/>
+      <c r="B68" s="61"/>
+      <c r="C68" s="61"/>
       <c r="D68" s="21"/>
       <c r="E68" s="26"/>
       <c r="F68" s="26"/>
-      <c r="G68" s="26"/>
-      <c r="H68" s="26"/>
+      <c r="G68" s="54"/>
+      <c r="H68" s="54"/>
       <c r="I68" s="15"/>
       <c r="J68" s="28"/>
       <c r="K68" s="29"/>
@@ -4518,13 +4756,13 @@
       <c r="A69" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="B69" s="21"/>
-      <c r="C69" s="21"/>
+      <c r="B69" s="61"/>
+      <c r="C69" s="61"/>
       <c r="D69" s="21"/>
       <c r="E69" s="22"/>
       <c r="F69" s="22"/>
-      <c r="G69" s="26"/>
-      <c r="H69" s="26"/>
+      <c r="G69" s="54"/>
+      <c r="H69" s="54"/>
       <c r="I69" s="15"/>
       <c r="J69" s="28"/>
       <c r="K69" s="29"/>
@@ -4550,13 +4788,13 @@
       <c r="A70" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B70" s="21"/>
-      <c r="C70" s="21"/>
+      <c r="B70" s="61"/>
+      <c r="C70" s="61"/>
       <c r="D70" s="21"/>
       <c r="E70" s="22"/>
       <c r="F70" s="22"/>
-      <c r="G70" s="26"/>
-      <c r="H70" s="26"/>
+      <c r="G70" s="54"/>
+      <c r="H70" s="54"/>
       <c r="I70" s="15"/>
       <c r="J70" s="28"/>
       <c r="K70" s="29"/>
@@ -4582,13 +4820,13 @@
       <c r="A71" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B71" s="21"/>
-      <c r="C71" s="21"/>
+      <c r="B71" s="61"/>
+      <c r="C71" s="61"/>
       <c r="D71" s="21"/>
       <c r="E71" s="26"/>
       <c r="F71" s="26"/>
-      <c r="G71" s="26"/>
-      <c r="H71" s="26"/>
+      <c r="G71" s="54"/>
+      <c r="H71" s="54"/>
       <c r="I71" s="15"/>
       <c r="J71" s="28"/>
       <c r="K71" s="29"/>
@@ -4614,13 +4852,13 @@
       <c r="A72" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B72" s="21"/>
-      <c r="C72" s="21"/>
+      <c r="B72" s="61"/>
+      <c r="C72" s="61"/>
       <c r="D72" s="21"/>
       <c r="E72" s="26"/>
       <c r="F72" s="26"/>
-      <c r="G72" s="26"/>
-      <c r="H72" s="26"/>
+      <c r="G72" s="54"/>
+      <c r="H72" s="54"/>
       <c r="I72" s="15"/>
       <c r="J72" s="28"/>
       <c r="K72" s="29"/>
@@ -4646,13 +4884,13 @@
       <c r="A73" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="B73" s="21"/>
-      <c r="C73" s="27"/>
+      <c r="B73" s="61"/>
+      <c r="C73" s="63"/>
       <c r="D73" s="27"/>
       <c r="E73" s="22"/>
       <c r="F73" s="26"/>
-      <c r="G73" s="26"/>
-      <c r="H73" s="26"/>
+      <c r="G73" s="54"/>
+      <c r="H73" s="54"/>
       <c r="I73" s="15"/>
       <c r="J73" s="28"/>
       <c r="K73" s="29"/>
@@ -4685,7 +4923,7 @@
     <mergeCell ref="A8:G8"/>
     <mergeCell ref="D5:F5"/>
   </mergeCells>
-  <conditionalFormatting sqref="J623:J747 J749 J751 J753 J755 J757 J759 J761 J763 J765:J771 J919:J1042 J1044:J1181 J1186:J1200 J1205:J1209 J1214:J1263 J1267:J1291 J1293:J1385 J1389:J1413 J1415:J1474 J1476:J1562 J1601:J1622 J1759:J1760 J1763:J1790 J1918:J1959 J1962:J1964 J1967 J1969:J1971 J1974:J2011 J2014:J2054 J2057:J2079 J2082:J2085 J2088 J2090:J2092 J2095:J2136 J2332:J65044 J9:J10 O623:O747 O749 O751 O753 O755 O757 O759 O761 O763 O765:O771 O919:O1042 O1044:O1181 O1186:O1200 O1205:O1209 O1214:O1263 O1267:O1291 O1293:O1385 O1389:O1413 O1415:O1474 O1476:O1562 O1601:O1622 O1759:O1760 O1763:O1790 O1918:O1959 O1962:O1964 O1967 O1969:O1971 O1974:O2011 O2014:O2054 O2057:O2079 O2082:O2085 O2088 O2090:O2092 O2095:O2136 O2332:O65044 O9:O10 O12:O606 J12:J606">
+  <conditionalFormatting sqref="J623:J747 J749 J751 J753 J755 J757 J759 J761 J763 J765:J771 J919:J1042 J1044:J1181 J1186:J1200 J1205:J1209 J1214:J1263 J1267:J1291 J1293:J1385 J1389:J1413 J1415:J1474 J1476:J1562 J1601:J1622 J1759:J1760 J1763:J1790 J1918:J1959 J1962:J1964 J1967 J1969:J1971 J1974:J2011 J2014:J2054 J2057:J2079 J2082:J2085 J2088 J2090:J2092 J2095:J2136 J2332:J65044 J9:J10 O623:O747 O749 O751 O753 O755 O757 O759 O761 O763 O765:O771 O919:O1042 O1044:O1181 O1186:O1200 O1205:O1209 O1214:O1263 O1267:O1291 O1293:O1385 O1389:O1413 O1415:O1474 O1476:O1562 O1601:O1622 O1759:O1760 O1763:O1790 O1918:O1959 O1962:O1964 O1967 O1969:O1971 O1974:O2011 O2014:O2054 O2057:O2079 O2082:O2085 O2088 O2090:O2092 O2095:O2136 O2332:O65044 O9:O10 O12:O606 J28:J606">
     <cfRule type="cellIs" dxfId="53" priority="75" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
@@ -4898,11 +5136,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="44.42578125" customWidth="1"/>
     <col min="5" max="5" width="43.140625" customWidth="1"/>
@@ -4962,25 +5200,25 @@
         <v>1</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>158</v>
-      </c>
-      <c r="C4" s="44">
+        <v>157</v>
+      </c>
+      <c r="C4" s="43">
         <v>44487</v>
       </c>
       <c r="D4" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="F4" s="21" t="s">
         <v>148</v>
-      </c>
-      <c r="E4" s="26" t="s">
-        <v>109</v>
-      </c>
-      <c r="F4" s="21" t="s">
-        <v>149</v>
       </c>
       <c r="G4" s="21" t="s">
         <v>97</v>
       </c>
       <c r="H4" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="96" x14ac:dyDescent="0.2">
@@ -4990,23 +5228,23 @@
       <c r="B5" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="44">
+      <c r="C5" s="43">
         <v>44487</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G5" s="21" t="s">
         <v>97</v>
       </c>
       <c r="H5" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="96" x14ac:dyDescent="0.2">
@@ -5016,23 +5254,23 @@
       <c r="B6" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="44">
+      <c r="C6" s="43">
         <v>44488</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G6" s="21" t="s">
         <v>97</v>
       </c>
       <c r="H6" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="84" x14ac:dyDescent="0.2">
@@ -5040,23 +5278,23 @@
         <v>4</v>
       </c>
       <c r="B7" s="21"/>
-      <c r="C7" s="44">
+      <c r="C7" s="43">
         <v>44488</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>153</v>
-      </c>
-      <c r="E7" s="46" t="s">
-        <v>136</v>
+        <v>152</v>
+      </c>
+      <c r="E7" s="45" t="s">
+        <v>135</v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G7" s="21" t="s">
         <v>97</v>
       </c>
       <c r="H7" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="24" x14ac:dyDescent="0.2">
@@ -5066,23 +5304,23 @@
       <c r="B8" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="44">
+      <c r="C8" s="43">
         <v>44488</v>
       </c>
       <c r="D8" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="E8" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="F8" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="G8" s="21" t="s">
         <v>156</v>
       </c>
-      <c r="G8" s="21" t="s">
-        <v>157</v>
-      </c>
       <c r="H8" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -5222,23 +5460,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A9EE5A02A2A6DC45B45E782DFEFDA45E" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7657f0a98c495c38e0a3edb0de0bfed3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="http://schemas.microsoft.com/sharepoint/v4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c79c8594d4fa4c9fd200c91a62336472" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v4"/>
@@ -5364,10 +5585,37 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44F5ECF4-AC36-4424-9554-2A768AEC1238}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1910A495-F8F1-4320-96F7-0EE9F01D3CE9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5383,19 +5631,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1910A495-F8F1-4320-96F7-0EE9F01D3CE9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44F5ECF4-AC36-4424-9554-2A768AEC1238}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>